<commit_message>
feat: add auto reply
</commit_message>
<xml_diff>
--- a/input/汇总_店铺.xlsx
+++ b/input/汇总_店铺.xlsx
@@ -478,6 +478,345 @@
       </c>
       <c r="C9"/>
     </row>
+    <row r="10" ht="25.5" customHeight="1">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>资料小铺</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.7fan38B?tk=WD5gfCUq3SV", "https://m.tb.cn/h.7fan38B?tk=WD5gfCUq3SV")</f>
+        <v>https://m.tb.cn/h.7fan38B?tk=WD5gfCUq3SV</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://m.tb.cn/h.7fan38B?tk=WD5gfCUq3SV</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="25.5" customHeight="1">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>路兮</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.7faHWPw?tk=WXOQfCUEeTG", "https://m.tb.cn/h.7faHWPw?tk=WXOQfCUEeTG")</f>
+        <v>https://m.tb.cn/h.7faHWPw?tk=WXOQfCUEeTG</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.7faHWPw?tk=WXOQfCUEeTG HU071 「路兮的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="25.5" customHeight="1">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>tb_136514646</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.7UeyCOY?tk=2YpTfC5ZI4E", "https://m.tb.cn/h.7UeyCOY?tk=2YpTfC5ZI4E")</f>
+        <v>https://m.tb.cn/h.7UeyCOY?tk=2YpTfC5ZI4E</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.7UeyCOY?tk=2YpTfC5ZI4E CZ193 「tb_136514646的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="25.5" customHeight="1">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>空谷画兰</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.74NtoYK?tk=JWjgfC5dr1q", "https://m.tb.cn/h.74NtoYK?tk=JWjgfC5dr1q")</f>
+        <v>https://m.tb.cn/h.74NtoYK?tk=JWjgfC5dr1q</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.74NtoYK?tk=JWjgfC5dr1q HU591 「空谷画兰的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="25.5" customHeight="1">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>心妍映雪</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.74NuTbH?tk=z2rNfC5Vrjp", "https://m.tb.cn/h.74NuTbH?tk=z2rNfC5Vrjp")</f>
+        <v>https://m.tb.cn/h.74NuTbH?tk=z2rNfC5Vrjp</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.74NuTbH?tk=z2rNfC5Vrjp CZ225 「心妍映雪的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="25.5" customHeight="1">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>BC素材铺</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.74NxfEu?tk=eg30fC55tdj", "https://m.tb.cn/h.74NxfEu?tk=eg30fC55tdj")</f>
+        <v>https://m.tb.cn/h.74NxfEu?tk=eg30fC55tdj</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.74NxfEu?tk=eg30fC55tdj HU926 「BC素材铺的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="25.5" customHeight="1">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>是啊花呀</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.7UVgR1r?tk=A2d0fC5S5AG", "https://m.tb.cn/h.7UVgR1r?tk=A2d0fC5S5AG")</f>
+        <v>https://m.tb.cn/h.7UVgR1r?tk=A2d0fC5S5AG</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.7UVgR1r?tk=A2d0fC5S5AG CZ193 「是啊花呀的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="25.5" customHeight="1">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>小狗资料铺</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.7fZgbLp?tk=VucMfC5Rh4q", "https://m.tb.cn/h.7fZgbLp?tk=VucMfC5Rh4q")</f>
+        <v>https://m.tb.cn/h.7fZgbLp?tk=VucMfC5Rh4q</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.7fZgbLp?tk=VucMfC5Rh4q CZ007 「小狗资料铺的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="25.5" customHeight="1">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>知二素材</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.74ndtH2?tk=INhpfC5lNVx", "https://m.tb.cn/h.74ndtH2?tk=INhpfC5lNVx")</f>
+        <v>https://m.tb.cn/h.74ndtH2?tk=INhpfC5lNVx</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.74ndtH2?tk=INhpfC5lNVx CZ356 「知二素材的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="25.5" customHeight="1">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>咕咕资源库</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.7fhgjkr?tk=mvsCfC5KhNt", "https://m.tb.cn/h.7fhgjkr?tk=mvsCfC5KhNt")</f>
+        <v>https://m.tb.cn/h.7fhgjkr?tk=mvsCfC5KhNt</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.7fhgjkr?tk=mvsCfC5KhNt HU287 「咕咕资源库的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="25.5" customHeight="1">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>基隆圆圆的苹果</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.74MYh6O?tk=9p9mfCgjX4S", "https://m.tb.cn/h.74MYh6O?tk=9p9mfCgjX4S")</f>
+        <v>https://m.tb.cn/h.74MYh6O?tk=9p9mfCgjX4S</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.74MYh6O?tk=9p9mfCgjX4S HU591 「基隆圆圆的苹果的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="25.5" customHeight="1">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>小北轻创业</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.74LZMia?tk=dXXSfC69dLZ", "https://m.tb.cn/h.74LZMia?tk=dXXSfC69dLZ")</f>
+        <v>https://m.tb.cn/h.74LZMia?tk=dXXSfC69dLZ</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.74LZMia?tk=dXXSfC69dLZ HU071 「小北轻创业的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="25.5" customHeight="1">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>卡布奇诺</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.74LYLg5?tk=nbazfC6OsxM", "https://m.tb.cn/h.74LYLg5?tk=nbazfC6OsxM")</f>
+        <v>https://m.tb.cn/h.74LYLg5?tk=nbazfC6OsxM</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.74LYLg5?tk=nbazfC6OsxM CZ193 「卡布奇诺的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" ht="25.5" customHeight="1">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>洋芋头的店</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.74LePlT?tk=m5LkfC6oqkG", "https://m.tb.cn/h.74LePlT?tk=m5LkfC6oqkG")</f>
+        <v>https://m.tb.cn/h.74LePlT?tk=m5LkfC6oqkG</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.74LePlT?tk=m5LkfC6oqkG MF278 「洋芋头的店的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="25.5" customHeight="1">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>怕黑的海龟</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.7UUqoxG?tk=VXX7fC6sGJL", "https://m.tb.cn/h.7UUqoxG?tk=VXX7fC6sGJL")</f>
+        <v>https://m.tb.cn/h.7UUqoxG?tk=VXX7fC6sGJL</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.7UUqoxG?tk=VXX7fC6sGJL CZ007 「怕黑的海龟的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="25.5" customHeight="1">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>森森资源小铺</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.7UUtWft?tk=QC8GfC6Flq1", "https://m.tb.cn/h.7UUtWft?tk=QC8GfC6Flq1")</f>
+        <v>https://m.tb.cn/h.7UUtWft?tk=QC8GfC6Flq1</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.7UUtWft?tk=QC8GfC6Flq1 CZ193 「森森资源小铺的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="25.5" customHeight="1">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>思秋云舒</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.7fYGf0W?tk=uVG5fC6Fv0L", "https://m.tb.cn/h.7fYGf0W?tk=uVG5fC6Fv0L")</f>
+        <v>https://m.tb.cn/h.7fYGf0W?tk=uVG5fC6Fv0L</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.7fYGf0W?tk=uVG5fC6Fv0L CZ009 「思秋云舒的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="25.5" customHeight="1">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>悠然资料铺</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.7UUwOQE?tk=XAXxfC6xs6E", "https://m.tb.cn/h.7UUwOQE?tk=XAXxfC6xs6E")</f>
+        <v>https://m.tb.cn/h.7UUwOQE?tk=XAXxfC6xs6E</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.7UUwOQE?tk=XAXxfC6xs6E CZ057 「悠然资料铺的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="25.5" customHeight="1">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Miao</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.7fYyTZn?tk=7yXIfC6zguE", "https://m.tb.cn/h.7fYyTZn?tk=7yXIfC6zguE")</f>
+        <v>https://m.tb.cn/h.7fYyTZn?tk=7yXIfC6zguE</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.7fYyTZn?tk=7yXIfC6zguE MF287 「Miao的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="25.5" customHeight="1">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>资料分享吧</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="str">
+        <f>=HYPERLINK("https://m.tb.cn/h.7f1Y5ed?tk=TVijfChXEep", "https://m.tb.cn/h.7f1Y5ed?tk=TVijfChXEep")</f>
+        <v>https://m.tb.cn/h.7f1Y5ed?tk=TVijfChXEep</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>【闲鱼】https://m.tb.cn/h.7f1Y5ed?tk=TVijfChXEep MF278 「资料分享吧的闲鱼号，快来关注TA吧～」
+点击链接直接打开</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>